<commit_message>
added images, extendet intro
</commit_message>
<xml_diff>
--- a/requirements/Requirements Excel/Requirement Error Logger.xlsx
+++ b/requirements/Requirements Excel/Requirement Error Logger.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repositories\Bird_Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repositories\Bird_Requirements\requirements\Requirements Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C92DE60-DF57-4B4F-B2E2-6606D4800992}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F3BAC5-5BD9-4A05-A9E4-98845B21CE2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02421E9F-6F91-4F88-92F9-C987603F6219}"/>
   </bookViews>
@@ -663,7 +663,7 @@
       <c r="D3" s="6"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:5" ht="91" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>

</xml_diff>